<commit_message>
Update OPER 785 HW1 - Hosley.xlsx
</commit_message>
<xml_diff>
--- a/2023Q3 - Machine Learning 2/HW1/OPER 785 HW1 - Hosley.xlsx
+++ b/2023Q3 - Machine Learning 2/HW1/OPER 785 HW1 - Hosley.xlsx
@@ -5,33 +5,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Single Output" sheetId="2" r:id="rId5"/>
-    <sheet name="homework 1" sheetId="3" r:id="rId6"/>
+    <sheet name="Single Output" sheetId="1" r:id="rId4"/>
+    <sheet name="homework 1" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
-  <si>
-    <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
-  </si>
-  <si>
-    <t>Numbers Sheet Name</t>
-  </si>
-  <si>
-    <t>Numbers Table Name</t>
-  </si>
-  <si>
-    <t>Excel Worksheet Name</t>
-  </si>
-  <si>
-    <t>Single Output</t>
-  </si>
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>x1</t>
   </si>
@@ -72,9 +53,6 @@
     <t>bias adjustment</t>
   </si>
   <si>
-    <t>homework 1</t>
-  </si>
-  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -92,19 +70,9 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -114,29 +82,17 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -146,13 +102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -167,14 +117,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -182,7 +132,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -190,28 +140,28 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -224,26 +174,26 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -252,13 +202,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thick">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -270,10 +220,10 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -282,22 +232,22 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thick">
         <color indexed="8"/>
@@ -306,7 +256,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -315,28 +265,28 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
       <right style="thick">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -345,13 +295,13 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -361,38 +311,23 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -401,13 +336,13 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -419,13 +354,13 @@
     <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -499,9 +434,6 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff5e88b1"/>
-      <rgbColor rgb="ffeef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ffffffff"/>
@@ -1536,516 +1468,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s" s="5">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D10" location="'Single Output'!R1C1" tooltip="" display="Single Output"/>
-    <hyperlink ref="D12" location="'homework 1'!R1C1" tooltip="" display="homework 1"/>
-  </hyperlinks>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.8516" style="6" customWidth="1"/>
-    <col min="3" max="4" width="4.17188" style="6" customWidth="1"/>
-    <col min="5" max="5" width="4.85156" style="6" customWidth="1"/>
-    <col min="6" max="6" width="5.17188" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.85156" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.67188" style="6" customWidth="1"/>
-    <col min="9" max="11" width="6.17188" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.3516" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="4" width="4.17188" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.17188" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.67188" style="1" customWidth="1"/>
+    <col min="9" max="11" width="6.17188" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.3516" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" t="s" s="8">
+      <c r="A1" s="2"/>
+      <c r="B1" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4">
+        <v>0</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="C1" s="9">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" t="s" s="8">
+      <c r="C7" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="F1" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" t="s" s="13">
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="C2" s="14">
-        <v>3</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" t="s" s="13">
+      <c r="G7" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C3" s="14">
-        <v>5</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="13">
+      <c r="H7" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="C5" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s" s="17">
+      <c r="I7" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="18">
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
-      <c r="L7" t="s" s="25">
-        <v>18</v>
-      </c>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="26">
-        <v>1</v>
-      </c>
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28">
-        <v>1</v>
-      </c>
-      <c r="D8" s="29">
-        <v>1</v>
-      </c>
-      <c r="E8" s="30">
-        <v>1</v>
-      </c>
-      <c r="F8" s="28">
+      <c r="A8" s="21">
+        <v>1</v>
+      </c>
+      <c r="B8" s="22">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+      <c r="F8" s="23">
         <v>10</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="21">
         <f>IF(F8&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="25">
         <f>$F$1-G8</f>
         <v>-1</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="23">
         <f>$C$5*$H8*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="24">
         <f>$C$5*$H8*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="25">
         <f>$C$5*$H8*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="23">
         <f>$C$5*$H8*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="31">
+      <c r="A9" s="26">
         <v>2</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="27">
         <f>B8+L8</f>
         <v>0.9</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="28">
         <f>C8+I8</f>
         <v>0.9</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="29">
         <f>D8+J8</f>
         <v>0.7</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="30">
         <f>E8+K8</f>
         <v>0.5</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="28">
         <f>B9+$C$1*C9+$C$2*D9+$C$3*E9</f>
         <v>6.4</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="26">
         <f>IF(F9&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="30">
         <f>$F$1-G9</f>
         <v>-1</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="28">
         <f>$C$5*$H9*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="29">
         <f>$C$5*$H9*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="30">
         <f>$C$5*$H9*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="28">
         <f>$C$5*$H9*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="31">
+      <c r="A10" s="26">
         <v>3</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="27">
         <f>B9+L9</f>
         <v>0.8</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="28">
         <f>C9+I9</f>
         <v>0.8</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="29">
         <f>D9+J9</f>
         <v>0.4</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="30">
         <f>E9+K9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="28">
         <f>B10+$C$1*C10+$C$2*D10+$C$3*E10</f>
         <v>2.8</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="26">
         <f>IF(F10&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="30">
         <f>$F$1-G10</f>
         <v>-1</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="28">
         <f>$C$5*$H10*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="29">
         <f>$C$5*$H10*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="30">
         <f>$C$5*$H10*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="28">
         <f>$C$5*$H10*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="31">
+      <c r="A11" s="26">
         <v>4</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="27">
         <f>B10+L10</f>
         <v>0.7</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="28">
         <f>C10+I10</f>
         <v>0.7</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="29">
         <f>D10+J10</f>
         <v>0.1</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="30">
         <f>E10+K10</f>
         <v>-0.5</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="28">
         <f>B11+$C$1*C11+$C$2*D11+$C$3*E11</f>
         <v>-0.8</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="26">
         <f>IF(F11&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="30">
         <f>$F$1-G11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="28">
         <f>$C$5*$H11*$C$1</f>
         <v>0</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="29">
         <f>$C$5*$H11*$C$2</f>
         <v>0</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="30">
         <f>$C$5*$H11*$C$3</f>
         <v>0</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="28">
         <f>$C$5*$H11*$B$8</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="31">
+      <c r="A12" s="26">
         <v>5</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="33"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="31">
+      <c r="A13" s="26">
         <v>6</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="33"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="31">
+      <c r="A14" s="26">
         <v>7</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="33"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="31">
+      <c r="A15" s="26">
         <v>8</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="33"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="31">
+      <c r="A16" s="26">
         <v>9</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="33"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="31">
+      <c r="A17" s="26">
         <v>10</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="33"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2060,7 +1920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:L32"/>
   <sheetViews>
@@ -2068,964 +1928,964 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="36" customWidth="1"/>
-    <col min="2" max="2" width="10.8516" style="36" customWidth="1"/>
-    <col min="3" max="4" width="4.17188" style="36" customWidth="1"/>
-    <col min="5" max="5" width="4.85156" style="36" customWidth="1"/>
-    <col min="6" max="6" width="5.17188" style="36" customWidth="1"/>
-    <col min="7" max="7" width="9.85156" style="36" customWidth="1"/>
-    <col min="8" max="8" width="8.67188" style="36" customWidth="1"/>
-    <col min="9" max="11" width="6.17188" style="36" customWidth="1"/>
-    <col min="12" max="12" width="13.3516" style="36" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="36" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="31" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="31" customWidth="1"/>
+    <col min="3" max="4" width="4.17188" style="31" customWidth="1"/>
+    <col min="5" max="5" width="4.85156" style="31" customWidth="1"/>
+    <col min="6" max="6" width="5.17188" style="31" customWidth="1"/>
+    <col min="7" max="7" width="9.85156" style="31" customWidth="1"/>
+    <col min="8" max="8" width="8.67188" style="31" customWidth="1"/>
+    <col min="9" max="11" width="6.17188" style="31" customWidth="1"/>
+    <col min="12" max="12" width="13.3516" style="31" customWidth="1"/>
+    <col min="13" max="16384" width="8.85156" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" t="s" s="8">
+      <c r="A1" s="2"/>
+      <c r="B1" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4">
+        <v>0</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="32">
+        <v>13</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="C1" s="9">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="F1" s="9">
-        <v>0</v>
-      </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" t="s" s="13">
+      <c r="C7" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="C2" s="14">
-        <v>3</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" t="s" s="13">
+      <c r="G7" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C3" s="14">
-        <v>5</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="13">
+      <c r="H7" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="C5" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="37">
-        <v>20</v>
-      </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s" s="17">
+      <c r="I7" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="18">
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
-      <c r="L7" t="s" s="25">
-        <v>18</v>
-      </c>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="26">
-        <v>1</v>
-      </c>
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28">
-        <v>1</v>
-      </c>
-      <c r="D8" s="29">
-        <v>1</v>
-      </c>
-      <c r="E8" s="30">
-        <v>1</v>
-      </c>
-      <c r="F8" s="28">
+      <c r="A8" s="21">
+        <v>1</v>
+      </c>
+      <c r="B8" s="22">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+      <c r="F8" s="23">
         <v>10</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="21">
         <f>IF(F8&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="25">
         <f>$F$1-G8</f>
         <v>-1</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="23">
         <f>$C$5*$H8*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="24">
         <f>$C$5*$H8*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="25">
         <f>$C$5*$H8*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="23">
         <f>$C$5*$H8*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="31">
+      <c r="A9" s="26">
         <v>2</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="27">
         <f>B8+L8</f>
         <v>0.9</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="28">
         <f>C8+I8</f>
         <v>0.9</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="29">
         <f>D8+J8</f>
         <v>0.7</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="30">
         <f>E8+K8</f>
         <v>0.5</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="28">
         <f>B9+$C$1*C9+$C$2*D9+$C$3*E9</f>
         <v>6.4</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="26">
         <f>IF(F9&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="30">
         <f>$F$1-G9</f>
         <v>-1</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="28">
         <f>$C$5*$H9*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="29">
         <f>$C$5*$H9*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="30">
         <f>$C$5*$H9*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="28">
         <f>$C$5*$H9*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="31">
+      <c r="A10" s="26">
         <v>3</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="27">
         <f>B9+L9</f>
         <v>0.8</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="28">
         <f>C9+I9</f>
         <v>0.8</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="29">
         <f>D9+J9</f>
         <v>0.4</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="30">
         <f>E9+K9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="28">
         <f>B10+$C$1*C10+$C$2*D10+$C$3*E10</f>
         <v>2.8</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="26">
         <f>IF(F10&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="30">
         <f>$F$1-G10</f>
         <v>-1</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="28">
         <f>$C$5*$H10*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="29">
         <f>$C$5*$H10*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="30">
         <f>$C$5*$H10*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="28">
         <f>$C$5*$H10*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="31">
+      <c r="A11" s="26">
         <v>4</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="27">
         <f>B10+L10</f>
         <v>0.7</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="28">
         <f>C10+I10</f>
         <v>0.7</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="29">
         <f>D10+J10</f>
         <v>0.1</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="30">
         <f>E10+K10</f>
         <v>-0.5</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="28">
         <f>B11+$C$1*C11+$C$2*D11+$C$3*E11</f>
         <v>-0.8</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="26">
         <f>IF(F11&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="30">
         <f>$F$1-G11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="28">
         <f>$C$5*$H11*$C$1</f>
         <v>0</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="29">
         <f>$C$5*$H11*$C$2</f>
         <v>0</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="30">
         <f>$C$5*$H11*$C$3</f>
         <v>0</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="28">
         <f>$C$5*$H11*$B$8</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="31">
+      <c r="A12" s="26">
         <v>5</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="33"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="31">
+      <c r="A13" s="26">
         <v>6</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="33"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="37">
-        <v>21</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
+      <c r="A15" t="s" s="32">
+        <v>14</v>
+      </c>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" t="s" s="17">
+      <c r="A16" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="B16" t="s" s="18">
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
+      <c r="L16" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="C16" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="H16" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="I16" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="24"/>
-      <c r="L16" t="s" s="25">
-        <v>18</v>
-      </c>
     </row>
     <row r="17" ht="14.05" customHeight="1">
-      <c r="A17" s="26">
-        <v>1</v>
-      </c>
-      <c r="B17" s="27">
-        <v>1</v>
-      </c>
-      <c r="C17" s="28">
-        <v>1</v>
-      </c>
-      <c r="D17" s="29">
-        <v>1</v>
-      </c>
-      <c r="E17" s="30">
-        <v>1</v>
-      </c>
-      <c r="F17" s="28">
+      <c r="A17" s="21">
+        <v>1</v>
+      </c>
+      <c r="B17" s="22">
+        <v>1</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1</v>
+      </c>
+      <c r="D17" s="24">
+        <v>1</v>
+      </c>
+      <c r="E17" s="25">
+        <v>1</v>
+      </c>
+      <c r="F17" s="23">
         <v>10</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="21">
         <f>IF(F17&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="25">
         <f>$F$2-G17</f>
         <v>-1</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="23">
         <f>$C$5*$H17*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="24">
         <f>$C$5*$H17*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="25">
         <f>$C$5*$H17*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L17" s="28">
+      <c r="L17" s="23">
         <f>$C$5*$H17*$B$17</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" s="31">
+      <c r="A18" s="26">
         <v>2</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="27">
         <f>B17+L17</f>
         <v>0.9</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="28">
         <f>C17+I17</f>
         <v>0.9</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="29">
         <f>D17+J17</f>
         <v>0.7</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="30">
         <f>E17+K17</f>
         <v>0.5</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="28">
         <f>B18+$C$1*C18+$C$2*D18+$C$3*E18</f>
         <v>6.4</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="26">
         <f>IF(F18&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="30">
         <f>$F$1-G18</f>
         <v>-1</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="28">
         <f>$C$5*$H18*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="29">
         <f>$C$5*$H18*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="30">
         <f>$C$5*$H18*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="28">
         <f>$C$5*$H18*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" s="31">
+      <c r="A19" s="26">
         <v>3</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="27">
         <f>B18+L18</f>
         <v>0.8</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="28">
         <f>C18+I18</f>
         <v>0.8</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="29">
         <f>D18+J18</f>
         <v>0.4</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="30">
         <f>E18+K18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="28">
         <f>B19+$C$1*C19+$C$2*D19+$C$3*E19</f>
         <v>2.8</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="26">
         <f>IF(F19&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H19" s="30">
         <f>$F$1-G19</f>
         <v>-1</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="28">
         <f>$C$5*$H19*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="29">
         <f>$C$5*$H19*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="30">
         <f>$C$5*$H19*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="28">
         <f>$C$5*$H19*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="31">
+      <c r="A20" s="26">
         <v>4</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="27">
         <f>B19+L19</f>
         <v>0.7</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="28">
         <f>C19+I19</f>
         <v>0.7</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="29">
         <f>D19+J19</f>
         <v>0.1</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="30">
         <f>E19+K19</f>
         <v>-0.5</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="28">
         <f>B20+$C$1*C20+$C$2*D20+$C$3*E20</f>
         <v>-0.8</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="26">
         <f>IF(F20&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H20" s="30">
         <f>$F$1-G20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="28">
         <f>$C$5*$H20*$C$1</f>
         <v>0</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J20" s="29">
         <f>$C$5*$H20*$C$2</f>
         <v>0</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="30">
         <f>$C$5*$H20*$C$3</f>
         <v>0</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="28">
         <f>$C$5*$H20*$B$8</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="31">
+      <c r="A21" s="26">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="33"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="28"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="31">
+      <c r="A22" s="26">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="33"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="28"/>
     </row>
     <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" t="s" s="37">
-        <v>22</v>
-      </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
+      <c r="A24" t="s" s="32">
+        <v>15</v>
+      </c>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" t="s" s="17">
+      <c r="A25" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="H25" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="B25" t="s" s="18">
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
+      <c r="L25" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="C25" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="G25" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="H25" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="I25" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="J25" s="23"/>
-      <c r="K25" s="24"/>
-      <c r="L25" t="s" s="25">
-        <v>18</v>
-      </c>
     </row>
     <row r="26" ht="14.05" customHeight="1">
-      <c r="A26" s="26">
-        <v>1</v>
-      </c>
-      <c r="B26" s="27">
-        <v>1</v>
-      </c>
-      <c r="C26" s="28">
-        <v>1</v>
-      </c>
-      <c r="D26" s="29">
-        <v>1</v>
-      </c>
-      <c r="E26" s="30">
-        <v>1</v>
-      </c>
-      <c r="F26" s="28">
+      <c r="A26" s="21">
+        <v>1</v>
+      </c>
+      <c r="B26" s="22">
+        <v>1</v>
+      </c>
+      <c r="C26" s="23">
+        <v>1</v>
+      </c>
+      <c r="D26" s="24">
+        <v>1</v>
+      </c>
+      <c r="E26" s="25">
+        <v>1</v>
+      </c>
+      <c r="F26" s="23">
         <v>10</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="21">
         <f>IF(F26&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="25">
         <f>$F$3-G26</f>
         <v>0</v>
       </c>
-      <c r="I26" s="28">
+      <c r="I26" s="23">
         <f>$C$5*$H26*$C$1</f>
         <v>0</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="24">
         <f>$C$5*$H26*$C$2</f>
         <v>0</v>
       </c>
-      <c r="K26" s="30">
+      <c r="K26" s="25">
         <f>$C$5*$H26*$C$3</f>
         <v>0</v>
       </c>
-      <c r="L26" s="28">
+      <c r="L26" s="23">
         <f>$C$5*$H26*$B$8</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" ht="13.55" customHeight="1">
-      <c r="A27" s="31">
+      <c r="A27" s="26">
         <v>2</v>
       </c>
-      <c r="B27" s="32">
+      <c r="B27" s="27">
         <f>B26+L26</f>
         <v>1</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="28">
         <f>C26+I26</f>
         <v>1</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="29">
         <f>D26+J26</f>
         <v>1</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="30">
         <f>E26+K26</f>
         <v>1</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="28">
         <f>B27+$C$1*C27+$C$2*D27+$C$3*E27</f>
         <v>10</v>
       </c>
-      <c r="G27" s="31">
+      <c r="G27" s="26">
         <f>IF(F27&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="30">
         <f>$F$1-G27</f>
         <v>-1</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I27" s="28">
         <f>$C$5*$H27*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="29">
         <f>$C$5*$H27*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="30">
         <f>$C$5*$H27*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L27" s="33">
+      <c r="L27" s="28">
         <f>$C$5*$H27*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" s="31">
+      <c r="A28" s="26">
         <v>3</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="27">
         <f>B27+L27</f>
         <v>0.9</v>
       </c>
-      <c r="C28" s="33">
+      <c r="C28" s="28">
         <f>C27+I27</f>
         <v>0.9</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="29">
         <f>D27+J27</f>
         <v>0.7</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E28" s="30">
         <f>E27+K27</f>
         <v>0.5</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="28">
         <f>B28+$C$1*C28+$C$2*D28+$C$3*E28</f>
         <v>6.4</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="26">
         <f>IF(F28&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="30">
         <f>$F$1-G28</f>
         <v>-1</v>
       </c>
-      <c r="I28" s="33">
+      <c r="I28" s="28">
         <f>$C$5*$H28*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="29">
         <f>$C$5*$H28*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="30">
         <f>$C$5*$H28*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L28" s="33">
+      <c r="L28" s="28">
         <f>$C$5*$H28*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" s="31">
+      <c r="A29" s="26">
         <v>4</v>
       </c>
-      <c r="B29" s="32">
+      <c r="B29" s="27">
         <f>B28+L28</f>
         <v>0.8</v>
       </c>
-      <c r="C29" s="33">
+      <c r="C29" s="28">
         <f>C28+I28</f>
         <v>0.8</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="29">
         <f>D28+J28</f>
         <v>0.4</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="30">
         <f>E28+K28</f>
         <v>0</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="28">
         <f>B29+$C$1*C29+$C$2*D29+$C$3*E29</f>
         <v>2.8</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="26">
         <f>IF(F29&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="30">
         <f>$F$1-G29</f>
         <v>-1</v>
       </c>
-      <c r="I29" s="33">
+      <c r="I29" s="28">
         <f>$C$5*$H29*$C$1</f>
         <v>-0.1</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="29">
         <f>$C$5*$H29*$C$2</f>
         <v>-0.3</v>
       </c>
-      <c r="K29" s="35">
+      <c r="K29" s="30">
         <f>$C$5*$H29*$C$3</f>
         <v>-0.5</v>
       </c>
-      <c r="L29" s="33">
+      <c r="L29" s="28">
         <f>$C$5*$H29*$B$8</f>
         <v>-0.1</v>
       </c>
     </row>
     <row r="30" ht="13.55" customHeight="1">
-      <c r="A30" s="31">
+      <c r="A30" s="26">
         <v>5</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="33"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="28"/>
     </row>
     <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" s="31">
+      <c r="A31" s="26">
         <v>6</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="33"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="28"/>
     </row>
     <row r="32" ht="13.55" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="33"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>